<commit_message>
assignment 2 is done
</commit_message>
<xml_diff>
--- a/references/src/assignment2/Problem6.xlsx
+++ b/references/src/assignment2/Problem6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\GitHub\csci-3200\references\src\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67D0B33-94E6-446F-A951-61429939C41B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28DCE317-36F9-4D09-9D0F-63957B2ED7FD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{272A0643-9F80-4FAB-B759-EB9ED5F094EF}"/>
   </bookViews>
@@ -2610,6 +2610,30 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>15625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>421875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1953125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3375000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5359375</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8000000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2835,6 +2859,573 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="79455648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>SummationSix</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Operations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$57:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$57:$B$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6137</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>17622</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23730</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31302</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9007-4429-9A49-EED4437366B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>O(N^2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$57:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$57:$C$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>625</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22500</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30625</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9007-4429-9A49-EED4437366B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$56</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>sum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$57:$A$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$57:$D$64</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1320</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2717</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3731</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6580</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9007-4429-9A49-EED4437366B9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="343977183"/>
+        <c:axId val="485140495"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="343977183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="485140495"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="485140495"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="343977183"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3114,6 +3705,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -5179,6 +5810,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5876,6 +7023,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B29B2948-0B5E-430C-952E-04FBCDB191F2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6178,8 +7361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B31C7AE-2623-436F-9856-3F91A5D5ECBD}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6712,6 +7895,10 @@
       <c r="B46">
         <v>4424854</v>
       </c>
+      <c r="C46">
+        <f>POWER(A46, 3)</f>
+        <v>15625</v>
+      </c>
       <c r="D46">
         <v>879060</v>
       </c>
@@ -6723,6 +7910,10 @@
       <c r="B47">
         <v>148683454</v>
       </c>
+      <c r="C47">
+        <f t="shared" ref="C47:C53" si="0">POWER(A47, 3)</f>
+        <v>125000</v>
+      </c>
       <c r="D47">
         <v>29688120</v>
       </c>
@@ -6734,6 +7925,10 @@
       <c r="B48">
         <v>1147807054</v>
       </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>421875</v>
+      </c>
       <c r="D48">
         <v>229395930</v>
       </c>
@@ -6745,6 +7940,10 @@
       <c r="B49">
         <v>4876983154</v>
       </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>1000000</v>
+      </c>
       <c r="D49">
         <v>975002490</v>
       </c>
@@ -6756,6 +7955,10 @@
       <c r="B50">
         <v>14957493004</v>
       </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>1953125</v>
+      </c>
       <c r="D50">
         <v>2990726550</v>
       </c>
@@ -6767,6 +7970,10 @@
       <c r="B51">
         <v>37342649104</v>
       </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>3375000</v>
+      </c>
       <c r="D51">
         <v>7467193110</v>
       </c>
@@ -6778,6 +7985,10 @@
       <c r="B52">
         <v>80903732704</v>
       </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>5359375</v>
+      </c>
       <c r="D52">
         <v>16178620920</v>
       </c>
@@ -6789,6 +8000,10 @@
       <c r="B53">
         <v>158015931304</v>
       </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>8000000</v>
+      </c>
       <c r="D53">
         <v>31600009980</v>
       </c>
@@ -6801,7 +8016,7 @@
         <v>1</v>
       </c>
       <c r="C56" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
         <v>5</v>
@@ -6814,6 +8029,9 @@
       <c r="B57">
         <v>780</v>
       </c>
+      <c r="C57">
+        <v>625</v>
+      </c>
       <c r="D57">
         <v>85</v>
       </c>
@@ -6825,6 +8043,9 @@
       <c r="B58">
         <v>4015</v>
       </c>
+      <c r="C58">
+        <v>2500</v>
+      </c>
       <c r="D58">
         <v>546</v>
       </c>
@@ -6836,6 +8057,9 @@
       <c r="B59">
         <v>6137</v>
       </c>
+      <c r="C59">
+        <v>5625</v>
+      </c>
       <c r="D59">
         <v>870</v>
       </c>
@@ -6847,6 +8071,9 @@
       <c r="B60">
         <v>9005</v>
       </c>
+      <c r="C60">
+        <v>10000</v>
+      </c>
       <c r="D60">
         <v>1320</v>
       </c>
@@ -6858,6 +8085,9 @@
       <c r="B61">
         <v>17622</v>
       </c>
+      <c r="C61">
+        <v>15625</v>
+      </c>
       <c r="D61">
         <v>2717</v>
       </c>
@@ -6869,6 +8099,9 @@
       <c r="B62">
         <v>23730</v>
       </c>
+      <c r="C62">
+        <v>22500</v>
+      </c>
       <c r="D62">
         <v>3731</v>
       </c>
@@ -6880,6 +8113,9 @@
       <c r="B63">
         <v>31302</v>
       </c>
+      <c r="C63">
+        <v>30625</v>
+      </c>
       <c r="D63">
         <v>5005</v>
       </c>
@@ -6890,6 +8126,9 @@
       </c>
       <c r="B64">
         <v>40555</v>
+      </c>
+      <c r="C64">
+        <v>40000</v>
       </c>
       <c r="D64">
         <v>6580</v>

</xml_diff>